<commit_message>
3 non decided are rejected ...but page can't be open so ....just kind of formality left
</commit_message>
<xml_diff>
--- a/organization.xlsx
+++ b/organization.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="21405"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="51120" windowHeight="26940" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="organization.csv" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="606" uniqueCount="594">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="607" uniqueCount="595">
   <si>
     <t>Key</t>
   </si>
@@ -1804,6 +1804,9 @@
   </si>
   <si>
     <t>only if no one else is applying</t>
+  </si>
+  <si>
+    <t>GDAL ...one project related to c++ implementation of filters</t>
   </si>
 </sst>
 </file>
@@ -1858,8 +1861,52 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="241">
+  <cellStyleXfs count="285">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -2105,7 +2152,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="241">
+  <cellStyles count="285">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -2226,6 +2273,28 @@
     <cellStyle name="Followed Hyperlink" xfId="236" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="238" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="240" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="242" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="244" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="246" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="248" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="250" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="252" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="254" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="256" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="258" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="260" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="262" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="264" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="266" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="268" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="270" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="272" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="274" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="276" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="278" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="280" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="282" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="284" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -2346,6 +2415,28 @@
     <cellStyle name="Hyperlink" xfId="235" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="237" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="239" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="241" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="243" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="245" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="247" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="249" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="251" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="253" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="255" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="257" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="259" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="261" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="263" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="265" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="267" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="269" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="271" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="273" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="275" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="277" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="279" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="281" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="283" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -2675,10 +2766,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L119"/>
+  <dimension ref="A1:L9"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="B68" sqref="B68"/>
+    <sheetView showRuler="0" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2688,7 +2779,7 @@
     <col min="3" max="3" width="249.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="25">
+    <row r="1" spans="1:12" ht="25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2702,279 +2793,54 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="25">
-      <c r="A2" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" ht="25">
-      <c r="A4" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" ht="25">
-      <c r="A13" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" ht="25">
-      <c r="A15" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="20" spans="1:12" ht="25">
-      <c r="A20" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="D20" s="1" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="26" spans="1:12" ht="25">
-      <c r="A26" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="B26" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="C26" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="D26" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="L26" t="s">
-        <v>555</v>
-      </c>
-    </row>
-    <row r="34" spans="1:12" ht="25">
-      <c r="A34" s="1" t="s">
-        <v>131</v>
-      </c>
-      <c r="B34" s="1" t="s">
-        <v>132</v>
-      </c>
-      <c r="C34" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="D34" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="L34" t="s">
-        <v>555</v>
-      </c>
-    </row>
-    <row r="36" spans="1:12" ht="25">
-      <c r="A36" s="1" t="s">
-        <v>139</v>
-      </c>
-      <c r="B36" s="1" t="s">
-        <v>140</v>
-      </c>
-      <c r="C36" s="1" t="s">
-        <v>141</v>
-      </c>
-      <c r="D36" s="1" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="40" spans="1:12" ht="25">
-      <c r="A40" s="1" t="s">
-        <v>155</v>
-      </c>
-      <c r="B40" s="1" t="s">
-        <v>156</v>
-      </c>
-      <c r="C40" s="1" t="s">
-        <v>157</v>
-      </c>
-      <c r="D40" s="1" t="s">
-        <v>158</v>
-      </c>
-      <c r="L40" t="s">
-        <v>555</v>
-      </c>
-    </row>
-    <row r="44" spans="1:12" ht="25">
-      <c r="A44" s="1" t="s">
-        <v>170</v>
-      </c>
-      <c r="B44" s="1" t="s">
-        <v>171</v>
-      </c>
-      <c r="C44" s="1" t="s">
-        <v>172</v>
-      </c>
-      <c r="D44" s="1" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="46" spans="1:12" ht="25">
-      <c r="A46" s="1" t="s">
-        <v>178</v>
-      </c>
-      <c r="B46" s="1" t="s">
-        <v>179</v>
-      </c>
-      <c r="C46" s="1" t="s">
-        <v>180</v>
-      </c>
-      <c r="D46" s="1" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="82" spans="1:12" ht="25">
-      <c r="A82" s="1" t="s">
-        <v>322</v>
-      </c>
-      <c r="B82" s="1" t="s">
-        <v>323</v>
-      </c>
-      <c r="C82" s="1" t="s">
-        <v>324</v>
-      </c>
-      <c r="D82" s="1" t="s">
-        <v>325</v>
-      </c>
-    </row>
-    <row r="90" spans="1:12" ht="25">
-      <c r="A90" s="1" t="s">
-        <v>354</v>
-      </c>
-      <c r="B90" s="1" t="s">
-        <v>355</v>
-      </c>
-      <c r="C90" s="1" t="s">
-        <v>356</v>
-      </c>
-      <c r="D90" s="1" t="s">
-        <v>357</v>
-      </c>
-    </row>
-    <row r="91" spans="1:12" ht="25">
-      <c r="A91" s="1" t="s">
-        <v>358</v>
-      </c>
-      <c r="B91" s="1" t="s">
-        <v>359</v>
-      </c>
-      <c r="C91" s="1" t="s">
-        <v>360</v>
-      </c>
-      <c r="D91" s="1" t="s">
-        <v>361</v>
-      </c>
-      <c r="L91" t="s">
+    <row r="7" spans="1:12" ht="25">
+      <c r="A7" s="1" t="s">
+        <v>394</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>395</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>396</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>397</v>
+      </c>
+      <c r="L7" t="s">
         <v>581</v>
       </c>
     </row>
-    <row r="100" spans="1:12" ht="25">
-      <c r="A100" s="1" t="s">
-        <v>394</v>
-      </c>
-      <c r="B100" s="1" t="s">
-        <v>395</v>
-      </c>
-      <c r="C100" s="1" t="s">
-        <v>396</v>
-      </c>
-      <c r="D100" s="1" t="s">
-        <v>397</v>
-      </c>
-      <c r="L100" t="s">
+    <row r="8" spans="1:12" ht="25">
+      <c r="A8" s="1" t="s">
+        <v>418</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>419</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>420</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>421</v>
+      </c>
+      <c r="L8" t="s">
         <v>581</v>
       </c>
     </row>
-    <row r="106" spans="1:12" ht="25">
-      <c r="A106" s="1" t="s">
-        <v>418</v>
-      </c>
-      <c r="B106" s="1" t="s">
-        <v>419</v>
-      </c>
-      <c r="C106" s="1" t="s">
-        <v>420</v>
-      </c>
-      <c r="D106" s="1" t="s">
-        <v>421</v>
-      </c>
-      <c r="L106" t="s">
-        <v>581</v>
-      </c>
-    </row>
-    <row r="112" spans="1:12" ht="25">
-      <c r="A112" s="1" t="s">
+    <row r="9" spans="1:12" ht="25">
+      <c r="A9" s="1" t="s">
         <v>441</v>
       </c>
-      <c r="B112" s="1" t="s">
+      <c r="B9" s="1" t="s">
         <v>442</v>
       </c>
-      <c r="C112" s="1" t="s">
+      <c r="C9" s="1" t="s">
         <v>443</v>
       </c>
-      <c r="D112" s="1" t="s">
+      <c r="D9" s="1" t="s">
         <v>444</v>
       </c>
-      <c r="L112" t="s">
-        <v>581</v>
-      </c>
-    </row>
-    <row r="119" spans="1:12" ht="25">
-      <c r="A119" s="1" t="s">
-        <v>469</v>
-      </c>
-      <c r="B119" s="1" t="s">
-        <v>470</v>
-      </c>
-      <c r="C119" s="1" t="s">
-        <v>471</v>
-      </c>
-      <c r="D119" s="1" t="s">
-        <v>472</v>
-      </c>
-      <c r="L119" t="s">
+      <c r="L9" t="s">
         <v>581</v>
       </c>
     </row>
@@ -3150,13 +3016,17 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S40"/>
+  <dimension ref="A1:S41"/>
   <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0">
-      <selection activeCell="N40" sqref="N40"/>
+    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
+      <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="2" max="2" width="77.6640625" customWidth="1"/>
+    <col min="3" max="3" width="157.1640625" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:19" ht="25">
       <c r="A1" s="1" t="s">
@@ -3817,6 +3687,23 @@
       </c>
       <c r="O40" t="s">
         <v>593</v>
+      </c>
+    </row>
+    <row r="41" spans="1:15" ht="25">
+      <c r="A41" s="1" t="s">
+        <v>322</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>323</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>324</v>
+      </c>
+      <c r="D41" s="1" t="s">
+        <v>325</v>
+      </c>
+      <c r="O41" t="s">
+        <v>594</v>
       </c>
     </row>
   </sheetData>
@@ -3831,10 +3718,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:X71"/>
+  <dimension ref="A1:X85"/>
   <sheetViews>
     <sheetView showRuler="0" topLeftCell="A45" workbookViewId="0">
-      <selection activeCell="A71" sqref="A71:XFD71"/>
+      <selection activeCell="A85" sqref="A85:XFD85"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -4851,6 +4738,217 @@
       </c>
       <c r="D71" s="1" t="s">
         <v>547</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" ht="25">
+      <c r="A72" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B72" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C72" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D72" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" ht="25">
+      <c r="A73" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B73" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C73" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D73" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" ht="25">
+      <c r="A74" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B74" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C74" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="D74" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" ht="25">
+      <c r="A75" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B75" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="C75" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="D75" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" ht="25">
+      <c r="A76" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="B76" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="C76" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="D76" s="1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" ht="25">
+      <c r="A77" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="B77" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="C77" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="D77" s="1" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" ht="25">
+      <c r="A78" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="B78" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="C78" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="D78" s="1" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" ht="25">
+      <c r="A79" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="B79" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="C79" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="D79" s="1" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" ht="25">
+      <c r="A80" s="1" t="s">
+        <v>354</v>
+      </c>
+      <c r="B80" s="1" t="s">
+        <v>355</v>
+      </c>
+      <c r="C80" s="1" t="s">
+        <v>356</v>
+      </c>
+      <c r="D80" s="1" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="81" spans="1:12" ht="25">
+      <c r="A81" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="B81" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="C81" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="D81" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="L81" t="s">
+        <v>555</v>
+      </c>
+    </row>
+    <row r="82" spans="1:12" ht="25">
+      <c r="A82" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="B82" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="C82" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="D82" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="L82" t="s">
+        <v>555</v>
+      </c>
+    </row>
+    <row r="83" spans="1:12" ht="25">
+      <c r="A83" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="B83" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="C83" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="D83" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="L83" t="s">
+        <v>555</v>
+      </c>
+    </row>
+    <row r="84" spans="1:12" ht="25">
+      <c r="A84" s="1" t="s">
+        <v>358</v>
+      </c>
+      <c r="B84" s="1" t="s">
+        <v>359</v>
+      </c>
+      <c r="C84" s="1" t="s">
+        <v>360</v>
+      </c>
+      <c r="D84" s="1" t="s">
+        <v>361</v>
+      </c>
+      <c r="L84" t="s">
+        <v>581</v>
+      </c>
+    </row>
+    <row r="85" spans="1:12" ht="25">
+      <c r="A85" s="1" t="s">
+        <v>469</v>
+      </c>
+      <c r="B85" s="1" t="s">
+        <v>470</v>
+      </c>
+      <c r="C85" s="1" t="s">
+        <v>471</v>
+      </c>
+      <c r="D85" s="1" t="s">
+        <v>472</v>
+      </c>
+      <c r="L85" t="s">
+        <v>581</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
basic filtering done ....time to contact mailing list
</commit_message>
<xml_diff>
--- a/organization.xlsx
+++ b/organization.xlsx
@@ -4,13 +4,15 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="21405"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="20" windowWidth="51200" windowHeight="26740" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="organization.csv" sheetId="1" r:id="rId1"/>
-    <sheet name="easy" sheetId="2" r:id="rId2"/>
+    <sheet name="rejected" sheetId="4" r:id="rId2"/>
     <sheet name="not rejected" sheetId="3" r:id="rId3"/>
-    <sheet name="rejected" sheetId="4" r:id="rId4"/>
+    <sheet name="easy" sheetId="2" r:id="rId4"/>
+    <sheet name="good projects" sheetId="5" r:id="rId5"/>
+    <sheet name="good projects but tough" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
@@ -22,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="607" uniqueCount="595">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="631" uniqueCount="617">
   <si>
     <t>Key</t>
   </si>
@@ -1807,6 +1809,72 @@
   </si>
   <si>
     <t>GDAL ...one project related to c++ implementation of filters</t>
+  </si>
+  <si>
+    <t>Contact person: John Pye</t>
+  </si>
+  <si>
+    <t>Level of difficulty: medium/high</t>
+  </si>
+  <si>
+    <t>Must know: partial derivatives, thermodynamics</t>
+  </si>
+  <si>
+    <t>Languages: C</t>
+  </si>
+  <si>
+    <t>Priority: High</t>
+  </si>
+  <si>
+    <t>Fast Interactive Machine Learning Enabled by GPUs</t>
+  </si>
+  <si>
+    <t>3d geometry</t>
+  </si>
+  <si>
+    <t>everything in c++</t>
+  </si>
+  <si>
+    <t>check for competition</t>
+  </si>
+  <si>
+    <t>only if no competition</t>
+  </si>
+  <si>
+    <t>project 3</t>
+  </si>
+  <si>
+    <t>Native iPad App using RoboVM ​http://www.robovm.org/ ¶</t>
+  </si>
+  <si>
+    <t>ask them for project priorities</t>
+  </si>
+  <si>
+    <t>if low competition</t>
+  </si>
+  <si>
+    <t>google glass</t>
+  </si>
+  <si>
+    <t>not so tough</t>
+  </si>
+  <si>
+    <t>Design and Implementation of a new source video from mobile phone (Android). 1</t>
+  </si>
+  <si>
+    <t>. PaGMO code reusability improvement - difficulty 4/5</t>
+  </si>
+  <si>
+    <t>if no competition</t>
+  </si>
+  <si>
+    <t>Port HPX to IOS</t>
+  </si>
+  <si>
+    <t>Hawkular - iOS/Android client</t>
+  </si>
+  <si>
+    <t>vigra java bindings</t>
   </si>
 </sst>
 </file>
@@ -1861,8 +1929,116 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="285">
+  <cellStyleXfs count="393">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -2152,7 +2328,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="285">
+  <cellStyles count="393">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -2295,6 +2471,60 @@
     <cellStyle name="Followed Hyperlink" xfId="280" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="282" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="284" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="286" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="288" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="290" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="292" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="294" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="296" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="298" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="300" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="302" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="304" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="306" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="308" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="310" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="312" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="314" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="316" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="318" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="320" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="322" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="324" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="326" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="328" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="330" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="332" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="334" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="336" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="338" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="340" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="342" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="344" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="346" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="348" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="350" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="352" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="354" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="356" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="358" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="360" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="362" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="364" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="366" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="368" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="370" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="372" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="374" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="376" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="378" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="380" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="382" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="384" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="386" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="388" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="390" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="392" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -2437,6 +2667,60 @@
     <cellStyle name="Hyperlink" xfId="279" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="281" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="283" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="285" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="287" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="289" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="291" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="293" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="295" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="297" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="299" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="301" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="303" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="305" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="307" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="309" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="311" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="313" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="315" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="317" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="319" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="321" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="323" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="325" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="327" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="329" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="331" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="333" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="335" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="337" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="339" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="341" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="343" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="345" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="347" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="349" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="351" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="353" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="355" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="357" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="359" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="361" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="363" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="365" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="367" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="369" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="371" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="373" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="375" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="377" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="379" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="381" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="383" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="385" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="387" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="389" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="391" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -2857,10 +3141,1710 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I8"/>
+  <dimension ref="A1:X113"/>
+  <sheetViews>
+    <sheetView showRuler="0" topLeftCell="A85" workbookViewId="0">
+      <selection activeCell="A113" sqref="A113:XFD113"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="2" max="2" width="42.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:18" ht="25">
+      <c r="A1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" ht="25">
+      <c r="A2" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" ht="25">
+      <c r="A3" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" ht="25">
+      <c r="A4" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="L4" t="s">
+        <v>550</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" ht="25">
+      <c r="A5" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" ht="25">
+      <c r="A6" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="M6" t="s">
+        <v>551</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" ht="25">
+      <c r="A7" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="Q7" t="s">
+        <v>553</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" ht="25">
+      <c r="A8" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" ht="25">
+      <c r="A9" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="R9" t="s">
+        <v>553</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18" ht="25">
+      <c r="A10" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18" ht="25">
+      <c r="A11" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18" ht="25">
+      <c r="A12" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18" ht="25">
+      <c r="A13" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18" ht="25">
+      <c r="A14" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="M14" t="s">
+        <v>553</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18" ht="25">
+      <c r="A15" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18" ht="25">
+      <c r="A16" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="17" spans="1:24" ht="25">
+      <c r="A17" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="18" spans="1:24" ht="25">
+      <c r="A18" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="19" spans="1:24" ht="25">
+      <c r="A19" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="20" spans="1:24" ht="25">
+      <c r="A20" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="C20" s="1"/>
+      <c r="D20" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="M20" t="s">
+        <v>557</v>
+      </c>
+    </row>
+    <row r="21" spans="1:24" ht="25">
+      <c r="A21" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="X21" t="s">
+        <v>560</v>
+      </c>
+    </row>
+    <row r="22" spans="1:24" ht="25">
+      <c r="A22" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="23" spans="1:24" ht="25">
+      <c r="A23" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="24" spans="1:24" ht="25">
+      <c r="A24" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="25" spans="1:24" ht="25">
+      <c r="A25" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="26" spans="1:24" ht="25">
+      <c r="A26" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>231</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="27" spans="1:24" ht="25">
+      <c r="A27" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="28" spans="1:24" ht="25">
+      <c r="A28" s="1" t="s">
+        <v>254</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>255</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>256</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="29" spans="1:24" ht="25">
+      <c r="A29" s="1" t="s">
+        <v>258</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>259</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>260</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="30" spans="1:24" ht="25">
+      <c r="A30" s="1" t="s">
+        <v>262</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>263</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>264</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="31" spans="1:24" ht="25">
+      <c r="A31" s="1" t="s">
+        <v>270</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>271</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>272</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="32" spans="1:24" ht="25">
+      <c r="A32" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>275</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>276</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12" ht="25">
+      <c r="A33" s="1" t="s">
+        <v>278</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>279</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>280</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12" ht="25">
+      <c r="A34" s="1" t="s">
+        <v>282</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>283</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>284</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12" ht="25">
+      <c r="A35" s="1" t="s">
+        <v>290</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>291</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>292</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>293</v>
+      </c>
+      <c r="L35" t="s">
+        <v>574</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12" ht="25">
+      <c r="A36" s="1" t="s">
+        <v>306</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>307</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>308</v>
+      </c>
+      <c r="D36" s="1" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12" ht="25">
+      <c r="A37" s="1" t="s">
+        <v>310</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>311</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>312</v>
+      </c>
+      <c r="D37" s="1" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="38" spans="1:12" ht="25">
+      <c r="A38" s="1" t="s">
+        <v>318</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>319</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>320</v>
+      </c>
+      <c r="D38" s="1" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="39" spans="1:12" ht="25">
+      <c r="A39" s="1" t="s">
+        <v>338</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>339</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>340</v>
+      </c>
+      <c r="D39" s="1" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="40" spans="1:12" ht="25">
+      <c r="A40" s="1" t="s">
+        <v>334</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>335</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>336</v>
+      </c>
+      <c r="D40" s="1" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="41" spans="1:12" ht="25">
+      <c r="A41" s="1" t="s">
+        <v>342</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>343</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>344</v>
+      </c>
+      <c r="D41" s="1" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="42" spans="1:12" ht="25">
+      <c r="A42" s="1" t="s">
+        <v>346</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>347</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>348</v>
+      </c>
+      <c r="D42" s="1" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="43" spans="1:12" ht="25">
+      <c r="A43" s="1" t="s">
+        <v>350</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>351</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>352</v>
+      </c>
+      <c r="D43" s="1" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="44" spans="1:12" ht="25">
+      <c r="A44" s="1" t="s">
+        <v>362</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>363</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>364</v>
+      </c>
+      <c r="D44" s="1" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="45" spans="1:12" ht="25">
+      <c r="A45" s="1" t="s">
+        <v>366</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>367</v>
+      </c>
+      <c r="C45" s="1" t="s">
+        <v>368</v>
+      </c>
+      <c r="D45" s="1" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="46" spans="1:12" ht="25">
+      <c r="A46" s="1" t="s">
+        <v>378</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>379</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>380</v>
+      </c>
+      <c r="D46" s="1" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="47" spans="1:12" ht="25">
+      <c r="A47" s="1" t="s">
+        <v>382</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>383</v>
+      </c>
+      <c r="C47" s="1" t="s">
+        <v>384</v>
+      </c>
+      <c r="D47" s="1" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="48" spans="1:12" ht="25">
+      <c r="A48" s="1" t="s">
+        <v>390</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>391</v>
+      </c>
+      <c r="C48" s="1" t="s">
+        <v>392</v>
+      </c>
+      <c r="D48" s="1" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" ht="25">
+      <c r="A49" s="1" t="s">
+        <v>398</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>399</v>
+      </c>
+      <c r="C49" s="1" t="s">
+        <v>400</v>
+      </c>
+      <c r="D49" s="1" t="s">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" ht="25">
+      <c r="A50" s="1" t="s">
+        <v>402</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>403</v>
+      </c>
+      <c r="C50" s="1" t="s">
+        <v>404</v>
+      </c>
+      <c r="D50" s="1" t="s">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" ht="25">
+      <c r="A51" s="1" t="s">
+        <v>406</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>407</v>
+      </c>
+      <c r="C51" s="1" t="s">
+        <v>408</v>
+      </c>
+      <c r="D51" s="1" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" ht="25">
+      <c r="A52" s="1" t="s">
+        <v>414</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>415</v>
+      </c>
+      <c r="C52" s="1" t="s">
+        <v>416</v>
+      </c>
+      <c r="D52" s="1" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" ht="25">
+      <c r="A53" s="1" t="s">
+        <v>422</v>
+      </c>
+      <c r="B53" s="1" t="s">
+        <v>423</v>
+      </c>
+      <c r="C53" s="1" t="s">
+        <v>424</v>
+      </c>
+      <c r="D53" s="1" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" ht="25">
+      <c r="A54" s="1" t="s">
+        <v>426</v>
+      </c>
+      <c r="B54" s="1" t="s">
+        <v>427</v>
+      </c>
+      <c r="C54" s="1" t="s">
+        <v>428</v>
+      </c>
+      <c r="D54" s="1" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" ht="25">
+      <c r="A55" s="1" t="s">
+        <v>433</v>
+      </c>
+      <c r="B55" s="1" t="s">
+        <v>434</v>
+      </c>
+      <c r="C55" s="1" t="s">
+        <v>435</v>
+      </c>
+      <c r="D55" s="1" t="s">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" ht="25">
+      <c r="A56" s="1" t="s">
+        <v>445</v>
+      </c>
+      <c r="B56" s="1" t="s">
+        <v>446</v>
+      </c>
+      <c r="C56" s="1" t="s">
+        <v>447</v>
+      </c>
+      <c r="D56" s="1" t="s">
+        <v>448</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" ht="25">
+      <c r="A57" s="1" t="s">
+        <v>453</v>
+      </c>
+      <c r="B57" s="1" t="s">
+        <v>454</v>
+      </c>
+      <c r="C57" s="1" t="s">
+        <v>455</v>
+      </c>
+      <c r="D57" s="1" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" ht="25">
+      <c r="A58" s="1" t="s">
+        <v>457</v>
+      </c>
+      <c r="B58" s="1" t="s">
+        <v>458</v>
+      </c>
+      <c r="C58" s="1" t="s">
+        <v>459</v>
+      </c>
+      <c r="D58" s="1" t="s">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" ht="25">
+      <c r="A59" s="1" t="s">
+        <v>461</v>
+      </c>
+      <c r="B59" s="1" t="s">
+        <v>462</v>
+      </c>
+      <c r="C59" s="1" t="s">
+        <v>463</v>
+      </c>
+      <c r="D59" s="1" t="s">
+        <v>464</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" ht="25">
+      <c r="A60" s="1" t="s">
+        <v>465</v>
+      </c>
+      <c r="B60" s="1" t="s">
+        <v>466</v>
+      </c>
+      <c r="C60" s="1" t="s">
+        <v>467</v>
+      </c>
+      <c r="D60" s="1" t="s">
+        <v>468</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" ht="25">
+      <c r="A61" s="1" t="s">
+        <v>473</v>
+      </c>
+      <c r="B61" s="1" t="s">
+        <v>474</v>
+      </c>
+      <c r="C61" s="1" t="s">
+        <v>475</v>
+      </c>
+      <c r="D61" s="1" t="s">
+        <v>476</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" ht="25">
+      <c r="A62" s="1" t="s">
+        <v>477</v>
+      </c>
+      <c r="B62" s="1" t="s">
+        <v>478</v>
+      </c>
+      <c r="C62" s="1"/>
+      <c r="D62" s="1" t="s">
+        <v>479</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" ht="25">
+      <c r="A63" s="1" t="s">
+        <v>480</v>
+      </c>
+      <c r="B63" s="1" t="s">
+        <v>481</v>
+      </c>
+      <c r="C63" s="1" t="s">
+        <v>482</v>
+      </c>
+      <c r="D63" s="1" t="s">
+        <v>483</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" ht="25">
+      <c r="A64" s="1" t="s">
+        <v>484</v>
+      </c>
+      <c r="B64" s="1" t="s">
+        <v>485</v>
+      </c>
+      <c r="C64" s="1" t="s">
+        <v>486</v>
+      </c>
+      <c r="D64" s="1" t="s">
+        <v>487</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" ht="25">
+      <c r="A65" s="1" t="s">
+        <v>492</v>
+      </c>
+      <c r="B65" s="1" t="s">
+        <v>493</v>
+      </c>
+      <c r="C65" s="1" t="s">
+        <v>494</v>
+      </c>
+      <c r="D65" s="1" t="s">
+        <v>495</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" ht="25">
+      <c r="A66" s="1" t="s">
+        <v>500</v>
+      </c>
+      <c r="B66" s="1" t="s">
+        <v>501</v>
+      </c>
+      <c r="C66" s="1" t="s">
+        <v>502</v>
+      </c>
+      <c r="D66" s="1" t="s">
+        <v>503</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" ht="25">
+      <c r="A67" s="1" t="s">
+        <v>508</v>
+      </c>
+      <c r="B67" s="1" t="s">
+        <v>509</v>
+      </c>
+      <c r="C67" s="1" t="s">
+        <v>510</v>
+      </c>
+      <c r="D67" s="1" t="s">
+        <v>511</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" ht="25">
+      <c r="A68" s="1" t="s">
+        <v>524</v>
+      </c>
+      <c r="B68" s="1" t="s">
+        <v>525</v>
+      </c>
+      <c r="C68" s="1" t="s">
+        <v>526</v>
+      </c>
+      <c r="D68" s="1" t="s">
+        <v>527</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" ht="25">
+      <c r="A69" s="1" t="s">
+        <v>528</v>
+      </c>
+      <c r="B69" s="1" t="s">
+        <v>529</v>
+      </c>
+      <c r="C69" s="1" t="s">
+        <v>530</v>
+      </c>
+      <c r="D69" s="1" t="s">
+        <v>531</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" ht="25">
+      <c r="A70" s="1" t="s">
+        <v>540</v>
+      </c>
+      <c r="B70" s="1" t="s">
+        <v>541</v>
+      </c>
+      <c r="C70" s="1" t="s">
+        <v>542</v>
+      </c>
+      <c r="D70" s="1" t="s">
+        <v>543</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" ht="25">
+      <c r="A71" s="1" t="s">
+        <v>544</v>
+      </c>
+      <c r="B71" s="1" t="s">
+        <v>545</v>
+      </c>
+      <c r="C71" s="1" t="s">
+        <v>546</v>
+      </c>
+      <c r="D71" s="1" t="s">
+        <v>547</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" ht="25">
+      <c r="A72" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B72" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C72" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D72" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" ht="25">
+      <c r="A73" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B73" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C73" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D73" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" ht="25">
+      <c r="A74" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B74" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C74" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="D74" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" ht="25">
+      <c r="A75" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B75" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="C75" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="D75" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" ht="25">
+      <c r="A76" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="B76" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="C76" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="D76" s="1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" ht="25">
+      <c r="A77" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="B77" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="C77" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="D77" s="1" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" ht="25">
+      <c r="A78" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="B78" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="C78" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="D78" s="1" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" ht="25">
+      <c r="A79" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="B79" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="C79" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="D79" s="1" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" ht="25">
+      <c r="A80" s="1" t="s">
+        <v>354</v>
+      </c>
+      <c r="B80" s="1" t="s">
+        <v>355</v>
+      </c>
+      <c r="C80" s="1" t="s">
+        <v>356</v>
+      </c>
+      <c r="D80" s="1" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="81" spans="1:19" ht="25">
+      <c r="A81" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="B81" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="C81" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="D81" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="L81" t="s">
+        <v>555</v>
+      </c>
+    </row>
+    <row r="82" spans="1:19" ht="25">
+      <c r="A82" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="B82" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="C82" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="D82" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="L82" t="s">
+        <v>555</v>
+      </c>
+    </row>
+    <row r="83" spans="1:19" ht="25">
+      <c r="A83" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="B83" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="C83" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="D83" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="L83" t="s">
+        <v>555</v>
+      </c>
+    </row>
+    <row r="84" spans="1:19" ht="25">
+      <c r="A84" s="1" t="s">
+        <v>358</v>
+      </c>
+      <c r="B84" s="1" t="s">
+        <v>359</v>
+      </c>
+      <c r="C84" s="1" t="s">
+        <v>360</v>
+      </c>
+      <c r="D84" s="1" t="s">
+        <v>361</v>
+      </c>
+      <c r="L84" t="s">
+        <v>581</v>
+      </c>
+    </row>
+    <row r="85" spans="1:19" ht="25">
+      <c r="A85" s="1" t="s">
+        <v>469</v>
+      </c>
+      <c r="B85" s="1" t="s">
+        <v>470</v>
+      </c>
+      <c r="C85" s="1" t="s">
+        <v>471</v>
+      </c>
+      <c r="D85" s="1" t="s">
+        <v>472</v>
+      </c>
+      <c r="L85" t="s">
+        <v>581</v>
+      </c>
+    </row>
+    <row r="91" spans="1:19" ht="25">
+      <c r="A91" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B91" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="C91" s="1"/>
+      <c r="D91" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="K91" t="s">
+        <v>552</v>
+      </c>
+    </row>
+    <row r="92" spans="1:19" ht="25">
+      <c r="A92" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="B92" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="C92" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="D92" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="M92" t="s">
+        <v>554</v>
+      </c>
+    </row>
+    <row r="93" spans="1:19" ht="25">
+      <c r="A93" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="B93" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="C93" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="D93" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="M93" t="s">
+        <v>557</v>
+      </c>
+    </row>
+    <row r="94" spans="1:19" ht="25">
+      <c r="A94" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="B94" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="C94" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="D94" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="S94" t="s">
+        <v>559</v>
+      </c>
+    </row>
+    <row r="95" spans="1:19" ht="25">
+      <c r="A95" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="B95" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="C95" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="D95" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="O95" t="s">
+        <v>565</v>
+      </c>
+    </row>
+    <row r="96" spans="1:19" ht="25">
+      <c r="A96" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="B96" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="C96" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="D96" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="O96" t="s">
+        <v>568</v>
+      </c>
+    </row>
+    <row r="97" spans="1:15" ht="25">
+      <c r="A97" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="B97" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="C97" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="D97" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="O97" t="s">
+        <v>569</v>
+      </c>
+    </row>
+    <row r="98" spans="1:15" ht="25">
+      <c r="A98" s="1" t="s">
+        <v>246</v>
+      </c>
+      <c r="B98" s="1" t="s">
+        <v>247</v>
+      </c>
+      <c r="C98" s="1" t="s">
+        <v>248</v>
+      </c>
+      <c r="D98" s="1" t="s">
+        <v>249</v>
+      </c>
+      <c r="O98" t="s">
+        <v>571</v>
+      </c>
+    </row>
+    <row r="99" spans="1:15" ht="25">
+      <c r="A99" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="B99" s="1" t="s">
+        <v>251</v>
+      </c>
+      <c r="C99" s="1" t="s">
+        <v>252</v>
+      </c>
+      <c r="D99" s="1" t="s">
+        <v>253</v>
+      </c>
+      <c r="O99" t="s">
+        <v>571</v>
+      </c>
+    </row>
+    <row r="100" spans="1:15" ht="25">
+      <c r="A100" s="1" t="s">
+        <v>294</v>
+      </c>
+      <c r="B100" s="1" t="s">
+        <v>295</v>
+      </c>
+      <c r="C100" s="1" t="s">
+        <v>296</v>
+      </c>
+      <c r="D100" s="1" t="s">
+        <v>297</v>
+      </c>
+      <c r="O100" t="s">
+        <v>575</v>
+      </c>
+    </row>
+    <row r="101" spans="1:15" ht="25">
+      <c r="A101" s="1" t="s">
+        <v>286</v>
+      </c>
+      <c r="B101" s="1" t="s">
+        <v>287</v>
+      </c>
+      <c r="C101" s="1" t="s">
+        <v>288</v>
+      </c>
+      <c r="D101" s="1" t="s">
+        <v>289</v>
+      </c>
+      <c r="O101" t="s">
+        <v>573</v>
+      </c>
+    </row>
+    <row r="102" spans="1:15" ht="25">
+      <c r="A102" s="1" t="s">
+        <v>314</v>
+      </c>
+      <c r="B102" s="1" t="s">
+        <v>315</v>
+      </c>
+      <c r="C102" s="1" t="s">
+        <v>316</v>
+      </c>
+      <c r="D102" s="1" t="s">
+        <v>317</v>
+      </c>
+      <c r="O102" t="s">
+        <v>578</v>
+      </c>
+    </row>
+    <row r="103" spans="1:15" ht="25">
+      <c r="A103" s="1" t="s">
+        <v>370</v>
+      </c>
+      <c r="B103" s="1" t="s">
+        <v>371</v>
+      </c>
+      <c r="C103" s="1" t="s">
+        <v>372</v>
+      </c>
+      <c r="D103" s="1" t="s">
+        <v>373</v>
+      </c>
+      <c r="O103" t="s">
+        <v>582</v>
+      </c>
+    </row>
+    <row r="104" spans="1:15" ht="25">
+      <c r="A104" s="1" t="s">
+        <v>410</v>
+      </c>
+      <c r="B104" s="1" t="s">
+        <v>411</v>
+      </c>
+      <c r="C104" s="1" t="s">
+        <v>412</v>
+      </c>
+      <c r="D104" s="1" t="s">
+        <v>413</v>
+      </c>
+      <c r="O104" t="s">
+        <v>554</v>
+      </c>
+    </row>
+    <row r="105" spans="1:15" ht="25">
+      <c r="A105" s="1" t="s">
+        <v>504</v>
+      </c>
+      <c r="B105" s="1" t="s">
+        <v>505</v>
+      </c>
+      <c r="C105" s="1" t="s">
+        <v>506</v>
+      </c>
+      <c r="D105" s="1" t="s">
+        <v>507</v>
+      </c>
+      <c r="O105" t="s">
+        <v>588</v>
+      </c>
+    </row>
+    <row r="106" spans="1:15" ht="25">
+      <c r="A106" s="1" t="s">
+        <v>488</v>
+      </c>
+      <c r="B106" s="1" t="s">
+        <v>489</v>
+      </c>
+      <c r="C106" s="1" t="s">
+        <v>490</v>
+      </c>
+      <c r="D106" s="1" t="s">
+        <v>491</v>
+      </c>
+      <c r="O106" t="s">
+        <v>587</v>
+      </c>
+    </row>
+    <row r="107" spans="1:15" ht="25">
+      <c r="A107" s="1" t="s">
+        <v>532</v>
+      </c>
+      <c r="B107" s="1" t="s">
+        <v>533</v>
+      </c>
+      <c r="C107" s="1" t="s">
+        <v>534</v>
+      </c>
+      <c r="D107" s="1" t="s">
+        <v>535</v>
+      </c>
+      <c r="O107" t="s">
+        <v>592</v>
+      </c>
+    </row>
+    <row r="108" spans="1:15" ht="25">
+      <c r="A108" s="1" t="s">
+        <v>536</v>
+      </c>
+      <c r="B108" s="1" t="s">
+        <v>537</v>
+      </c>
+      <c r="C108" s="1" t="s">
+        <v>538</v>
+      </c>
+      <c r="D108" s="1" t="s">
+        <v>539</v>
+      </c>
+      <c r="O108" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="109" spans="1:15" ht="25">
+      <c r="A109" s="1" t="s">
+        <v>437</v>
+      </c>
+      <c r="B109" s="1" t="s">
+        <v>438</v>
+      </c>
+      <c r="C109" s="1" t="s">
+        <v>439</v>
+      </c>
+      <c r="D109" s="1" t="s">
+        <v>440</v>
+      </c>
+      <c r="I109" t="s">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="112" spans="1:15" ht="25">
+      <c r="A112" s="1" t="s">
+        <v>374</v>
+      </c>
+      <c r="B112" s="1" t="s">
+        <v>375</v>
+      </c>
+      <c r="C112" s="1" t="s">
+        <v>376</v>
+      </c>
+      <c r="D112" s="1" t="s">
+        <v>377</v>
+      </c>
+      <c r="O112" t="s">
+        <v>583</v>
+      </c>
+    </row>
+    <row r="113" spans="1:15" ht="25">
+      <c r="A113" s="1" t="s">
+        <v>266</v>
+      </c>
+      <c r="B113" s="1" t="s">
+        <v>267</v>
+      </c>
+      <c r="C113" s="1" t="s">
+        <v>268</v>
+      </c>
+      <c r="D113" s="1" t="s">
+        <v>269</v>
+      </c>
+      <c r="O113" t="s">
+        <v>572</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:Q8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
+      <selection activeCell="B42" sqref="B42"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="2" max="2" width="77.6640625" customWidth="1"/>
+    <col min="3" max="3" width="157.1640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:17" ht="25">
+      <c r="A1" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="O1" t="s">
+        <v>561</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" ht="25">
+      <c r="A2" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="O2" t="s">
+        <v>562</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" ht="25">
+      <c r="A3" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="O3" t="s">
+        <v>564</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" ht="25">
+      <c r="A8" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>239</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="O8" t="s">
+        <v>570</v>
+      </c>
+      <c r="Q8" t="s">
+        <v>616</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:V21"/>
   <sheetViews>
     <sheetView showRuler="0" workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2871,7 +4855,7 @@
     <col min="4" max="4" width="82.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="25">
+    <row r="1" spans="1:10" ht="25">
       <c r="A1" s="1" t="s">
         <v>8</v>
       </c>
@@ -2888,7 +4872,7 @@
         <v>548</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="25">
+    <row r="2" spans="1:10" ht="25">
       <c r="A2" s="1" t="s">
         <v>52</v>
       </c>
@@ -2902,7 +4886,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="25">
+    <row r="3" spans="1:10" ht="25">
       <c r="A3" s="1" t="s">
         <v>123</v>
       </c>
@@ -2919,7 +4903,7 @@
         <v>556</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="25">
+    <row r="4" spans="1:10" ht="25">
       <c r="A4" s="1" t="s">
         <v>206</v>
       </c>
@@ -2935,8 +4919,11 @@
       <c r="F4" s="1" t="s">
         <v>566</v>
       </c>
-    </row>
-    <row r="5" spans="1:9" ht="25">
+      <c r="J4" t="s">
+        <v>615</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" ht="25">
       <c r="A5" s="1" t="s">
         <v>302</v>
       </c>
@@ -2953,24 +4940,7 @@
         <v>577</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="25">
-      <c r="A6" s="1" t="s">
-        <v>437</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>438</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>439</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>440</v>
-      </c>
-      <c r="I6" t="s">
-        <v>585</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" ht="25">
+    <row r="7" spans="1:10" ht="25">
       <c r="A7" s="1" t="s">
         <v>449</v>
       </c>
@@ -2987,7 +4957,7 @@
         <v>586</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="25">
+    <row r="8" spans="1:10" ht="25">
       <c r="A8" s="1" t="s">
         <v>520</v>
       </c>
@@ -3002,6 +4972,299 @@
       </c>
       <c r="I8" t="s">
         <v>591</v>
+      </c>
+    </row>
+    <row r="20" spans="1:22" ht="25">
+      <c r="A20" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="S20" t="s">
+        <v>563</v>
+      </c>
+      <c r="V20" t="s">
+        <v>606</v>
+      </c>
+    </row>
+    <row r="21" spans="1:22" ht="25">
+      <c r="A21" s="1" t="s">
+        <v>516</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>517</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>518</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>519</v>
+      </c>
+      <c r="O21" t="s">
+        <v>590</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:X37"/>
+  <sheetViews>
+    <sheetView showRuler="0" workbookViewId="0">
+      <selection activeCell="F46" sqref="F46"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="2" max="2" width="55.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:18" ht="25">
+      <c r="A1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="N1" t="s">
+        <v>599</v>
+      </c>
+      <c r="O1" t="s">
+        <v>598</v>
+      </c>
+      <c r="P1" t="s">
+        <v>595</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>596</v>
+      </c>
+      <c r="R1" t="s">
+        <v>597</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" ht="25">
+      <c r="A2" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="J2" t="s">
+        <v>549</v>
+      </c>
+      <c r="M2" t="s">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" ht="25">
+      <c r="A3" s="1" t="s">
+        <v>326</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>327</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>328</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>329</v>
+      </c>
+      <c r="O3" t="s">
+        <v>579</v>
+      </c>
+      <c r="R3" t="s">
+        <v>611</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" ht="25">
+      <c r="A4" s="1" t="s">
+        <v>386</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>387</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>388</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>389</v>
+      </c>
+      <c r="O4" t="s">
+        <v>584</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" ht="25">
+      <c r="A5" s="1" t="s">
+        <v>322</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>323</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>324</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>325</v>
+      </c>
+      <c r="O5" t="s">
+        <v>594</v>
+      </c>
+    </row>
+    <row r="32" spans="1:15" ht="25">
+      <c r="A32" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="M32" t="s">
+        <v>602</v>
+      </c>
+      <c r="O32" t="s">
+        <v>603</v>
+      </c>
+    </row>
+    <row r="33" spans="1:24" ht="25">
+      <c r="A33" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="M33" t="s">
+        <v>604</v>
+      </c>
+    </row>
+    <row r="34" spans="1:24" ht="25">
+      <c r="A34" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="S34" t="s">
+        <v>558</v>
+      </c>
+      <c r="V34" t="s">
+        <v>605</v>
+      </c>
+      <c r="X34" t="s">
+        <v>604</v>
+      </c>
+    </row>
+    <row r="35" spans="1:24" ht="25">
+      <c r="A35" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="O35" t="s">
+        <v>567</v>
+      </c>
+      <c r="S35" t="s">
+        <v>607</v>
+      </c>
+      <c r="V35" t="s">
+        <v>608</v>
+      </c>
+      <c r="X35" t="s">
+        <v>609</v>
+      </c>
+    </row>
+    <row r="36" spans="1:24" ht="25">
+      <c r="A36" s="1" t="s">
+        <v>330</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>331</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>332</v>
+      </c>
+      <c r="D36" s="1" t="s">
+        <v>333</v>
+      </c>
+      <c r="O36" t="s">
+        <v>580</v>
+      </c>
+      <c r="R36" t="s">
+        <v>612</v>
+      </c>
+      <c r="X36" t="s">
+        <v>613</v>
+      </c>
+    </row>
+    <row r="37" spans="1:24" ht="25">
+      <c r="A37" s="1" t="s">
+        <v>496</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>497</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>498</v>
+      </c>
+      <c r="D37" s="1" t="s">
+        <v>499</v>
+      </c>
+      <c r="O37" t="s">
+        <v>614</v>
+      </c>
+      <c r="X37" t="s">
+        <v>608</v>
       </c>
     </row>
   </sheetData>
@@ -3014,696 +5277,88 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S41"/>
+  <dimension ref="A1:R32"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+    <sheetView showRuler="0" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="2" max="2" width="77.6640625" customWidth="1"/>
-    <col min="3" max="3" width="157.1640625" customWidth="1"/>
+    <col min="2" max="2" width="53.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" ht="25">
+    <row r="1" spans="1:18" ht="25">
       <c r="A1" s="1" t="s">
-        <v>16</v>
+        <v>44</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>17</v>
+        <v>45</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>18</v>
+        <v>46</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="2" spans="1:19" ht="25">
+        <v>47</v>
+      </c>
+      <c r="R1" t="s">
+        <v>601</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" ht="25">
       <c r="A2" s="1" t="s">
-        <v>32</v>
+        <v>430</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>34</v>
-      </c>
+        <v>431</v>
+      </c>
+      <c r="C2" s="1"/>
       <c r="D2" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="J2" t="s">
-        <v>549</v>
-      </c>
-    </row>
-    <row r="3" spans="1:19" ht="25">
-      <c r="A3" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="4" spans="1:19" ht="25">
-      <c r="A4" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="5" spans="1:19" ht="25">
-      <c r="A5" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="C5" s="1"/>
-      <c r="D5" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="K5" t="s">
-        <v>552</v>
-      </c>
-    </row>
-    <row r="6" spans="1:19" ht="25">
-      <c r="A6" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="7" spans="1:19" ht="25">
-      <c r="A7" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>121</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="M7" t="s">
-        <v>554</v>
-      </c>
-    </row>
-    <row r="8" spans="1:19" ht="25">
-      <c r="A8" s="1" t="s">
-        <v>143</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>144</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>145</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>146</v>
-      </c>
-      <c r="M8" t="s">
+        <v>432</v>
+      </c>
+      <c r="O2" t="s">
         <v>557</v>
       </c>
     </row>
-    <row r="9" spans="1:19" ht="25">
-      <c r="A9" s="1" t="s">
-        <v>151</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>152</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>153</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>154</v>
-      </c>
-      <c r="S9" t="s">
-        <v>558</v>
-      </c>
-    </row>
-    <row r="10" spans="1:19" ht="25">
-      <c r="A10" s="1" t="s">
-        <v>159</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>160</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>161</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>162</v>
-      </c>
-      <c r="S10" t="s">
-        <v>559</v>
-      </c>
-    </row>
-    <row r="11" spans="1:19" ht="25">
-      <c r="A11" s="1" t="s">
-        <v>186</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>187</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>188</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>189</v>
-      </c>
-      <c r="S11" t="s">
-        <v>561</v>
-      </c>
-    </row>
-    <row r="12" spans="1:19" ht="25">
-      <c r="A12" s="1" t="s">
-        <v>190</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>191</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>192</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>193</v>
-      </c>
-      <c r="S12" t="s">
-        <v>562</v>
-      </c>
-    </row>
-    <row r="13" spans="1:19" ht="25">
-      <c r="A13" s="1" t="s">
-        <v>194</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>195</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>196</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>197</v>
-      </c>
-      <c r="S13" t="s">
-        <v>563</v>
-      </c>
-    </row>
-    <row r="14" spans="1:19" ht="25">
-      <c r="A14" s="1" t="s">
-        <v>198</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>199</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>200</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>201</v>
-      </c>
-      <c r="S14" t="s">
-        <v>564</v>
-      </c>
-    </row>
-    <row r="15" spans="1:19" ht="25">
-      <c r="A15" s="1" t="s">
-        <v>202</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>203</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>204</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>205</v>
-      </c>
-      <c r="O15" t="s">
-        <v>565</v>
-      </c>
-    </row>
-    <row r="16" spans="1:19" ht="25">
-      <c r="A16" s="1" t="s">
-        <v>210</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>211</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>212</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>213</v>
-      </c>
-      <c r="O16" t="s">
-        <v>567</v>
-      </c>
-    </row>
-    <row r="17" spans="1:15" ht="25">
-      <c r="A17" s="1" t="s">
-        <v>218</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>219</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>220</v>
-      </c>
-      <c r="D17" s="1" t="s">
-        <v>221</v>
-      </c>
-      <c r="O17" t="s">
-        <v>568</v>
-      </c>
-    </row>
-    <row r="18" spans="1:15" ht="25">
-      <c r="A18" s="1" t="s">
-        <v>226</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>227</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>228</v>
-      </c>
-      <c r="D18" s="1" t="s">
-        <v>229</v>
-      </c>
-      <c r="O18" t="s">
-        <v>569</v>
-      </c>
-    </row>
-    <row r="19" spans="1:15" ht="25">
-      <c r="A19" s="1" t="s">
-        <v>238</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>239</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>240</v>
-      </c>
-      <c r="D19" s="1" t="s">
-        <v>241</v>
-      </c>
-      <c r="O19" t="s">
-        <v>570</v>
-      </c>
-    </row>
-    <row r="20" spans="1:15" ht="25">
-      <c r="A20" s="1" t="s">
-        <v>246</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>247</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>248</v>
-      </c>
-      <c r="D20" s="1" t="s">
-        <v>249</v>
-      </c>
-      <c r="O20" t="s">
-        <v>571</v>
-      </c>
-    </row>
-    <row r="21" spans="1:15" ht="25">
-      <c r="A21" s="1" t="s">
-        <v>250</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>251</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>252</v>
-      </c>
-      <c r="D21" s="1" t="s">
-        <v>253</v>
-      </c>
-      <c r="O21" t="s">
-        <v>571</v>
-      </c>
-    </row>
-    <row r="22" spans="1:15" ht="25">
-      <c r="A22" s="1" t="s">
-        <v>266</v>
-      </c>
-      <c r="B22" s="1" t="s">
-        <v>267</v>
-      </c>
-      <c r="C22" s="1" t="s">
-        <v>268</v>
-      </c>
-      <c r="D22" s="1" t="s">
-        <v>269</v>
-      </c>
-      <c r="O22" t="s">
-        <v>572</v>
-      </c>
-    </row>
-    <row r="23" spans="1:15" ht="25">
-      <c r="A23" s="1" t="s">
-        <v>286</v>
-      </c>
-      <c r="B23" s="1" t="s">
-        <v>287</v>
-      </c>
-      <c r="C23" s="1" t="s">
-        <v>288</v>
-      </c>
-      <c r="D23" s="1" t="s">
-        <v>289</v>
-      </c>
-      <c r="O23" t="s">
-        <v>573</v>
-      </c>
-    </row>
-    <row r="24" spans="1:15" ht="25">
-      <c r="A24" s="1" t="s">
-        <v>294</v>
-      </c>
-      <c r="B24" s="1" t="s">
-        <v>295</v>
-      </c>
-      <c r="C24" s="1" t="s">
-        <v>296</v>
-      </c>
-      <c r="D24" s="1" t="s">
-        <v>297</v>
-      </c>
-      <c r="O24" t="s">
-        <v>575</v>
-      </c>
-    </row>
-    <row r="25" spans="1:15" ht="25">
-      <c r="A25" s="1" t="s">
-        <v>298</v>
-      </c>
-      <c r="B25" s="1" t="s">
-        <v>299</v>
-      </c>
-      <c r="C25" s="1" t="s">
-        <v>300</v>
-      </c>
-      <c r="D25" s="1" t="s">
-        <v>301</v>
-      </c>
-      <c r="O25" t="s">
-        <v>576</v>
-      </c>
-    </row>
-    <row r="26" spans="1:15" ht="25">
-      <c r="A26" s="1" t="s">
-        <v>314</v>
-      </c>
-      <c r="B26" s="1" t="s">
-        <v>315</v>
-      </c>
-      <c r="C26" s="1" t="s">
-        <v>316</v>
-      </c>
-      <c r="D26" s="1" t="s">
-        <v>317</v>
-      </c>
-      <c r="O26" t="s">
-        <v>578</v>
-      </c>
-    </row>
-    <row r="27" spans="1:15" ht="25">
-      <c r="A27" s="1" t="s">
-        <v>326</v>
-      </c>
-      <c r="B27" s="1" t="s">
-        <v>327</v>
-      </c>
-      <c r="C27" s="1" t="s">
-        <v>328</v>
-      </c>
-      <c r="D27" s="1" t="s">
-        <v>329</v>
-      </c>
-      <c r="O27" t="s">
-        <v>579</v>
-      </c>
-    </row>
-    <row r="28" spans="1:15" ht="25">
-      <c r="A28" s="1" t="s">
-        <v>330</v>
-      </c>
-      <c r="B28" s="1" t="s">
-        <v>331</v>
-      </c>
-      <c r="C28" s="1" t="s">
-        <v>332</v>
-      </c>
-      <c r="D28" s="1" t="s">
-        <v>333</v>
-      </c>
-      <c r="O28" t="s">
-        <v>580</v>
-      </c>
-    </row>
-    <row r="29" spans="1:15" ht="25">
-      <c r="A29" s="1" t="s">
-        <v>370</v>
-      </c>
-      <c r="B29" s="1" t="s">
-        <v>371</v>
-      </c>
-      <c r="C29" s="1" t="s">
-        <v>372</v>
-      </c>
-      <c r="D29" s="1" t="s">
-        <v>373</v>
-      </c>
-      <c r="O29" t="s">
-        <v>582</v>
-      </c>
-    </row>
-    <row r="30" spans="1:15" ht="25">
-      <c r="A30" s="1" t="s">
-        <v>374</v>
-      </c>
-      <c r="B30" s="1" t="s">
-        <v>375</v>
-      </c>
-      <c r="C30" s="1" t="s">
-        <v>376</v>
-      </c>
-      <c r="D30" s="1" t="s">
-        <v>377</v>
-      </c>
-      <c r="O30" t="s">
-        <v>583</v>
+    <row r="29" spans="1:15">
+      <c r="A29" t="s">
+        <v>610</v>
       </c>
     </row>
     <row r="31" spans="1:15" ht="25">
       <c r="A31" s="1" t="s">
-        <v>386</v>
+        <v>298</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>387</v>
+        <v>299</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>388</v>
+        <v>300</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>389</v>
+        <v>301</v>
       </c>
       <c r="O31" t="s">
-        <v>584</v>
+        <v>576</v>
       </c>
     </row>
     <row r="32" spans="1:15" ht="25">
       <c r="A32" s="1" t="s">
-        <v>410</v>
+        <v>512</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>411</v>
+        <v>513</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>412</v>
+        <v>514</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>413</v>
+        <v>515</v>
       </c>
       <c r="O32" t="s">
-        <v>554</v>
-      </c>
-    </row>
-    <row r="33" spans="1:15" ht="25">
-      <c r="A33" s="1" t="s">
-        <v>430</v>
-      </c>
-      <c r="B33" s="1" t="s">
-        <v>431</v>
-      </c>
-      <c r="C33" s="1"/>
-      <c r="D33" s="1" t="s">
-        <v>432</v>
-      </c>
-      <c r="O33" t="s">
-        <v>557</v>
-      </c>
-    </row>
-    <row r="34" spans="1:15" ht="25">
-      <c r="A34" s="1" t="s">
-        <v>488</v>
-      </c>
-      <c r="B34" s="1" t="s">
-        <v>489</v>
-      </c>
-      <c r="C34" s="1" t="s">
-        <v>490</v>
-      </c>
-      <c r="D34" s="1" t="s">
-        <v>491</v>
-      </c>
-      <c r="O34" t="s">
-        <v>587</v>
-      </c>
-    </row>
-    <row r="35" spans="1:15" ht="25">
-      <c r="A35" s="1" t="s">
-        <v>496</v>
-      </c>
-      <c r="B35" s="1" t="s">
-        <v>497</v>
-      </c>
-      <c r="C35" s="1" t="s">
-        <v>498</v>
-      </c>
-      <c r="D35" s="1" t="s">
-        <v>499</v>
-      </c>
-    </row>
-    <row r="36" spans="1:15" ht="25">
-      <c r="A36" s="1" t="s">
-        <v>504</v>
-      </c>
-      <c r="B36" s="1" t="s">
-        <v>505</v>
-      </c>
-      <c r="C36" s="1" t="s">
-        <v>506</v>
-      </c>
-      <c r="D36" s="1" t="s">
-        <v>507</v>
-      </c>
-      <c r="O36" t="s">
-        <v>588</v>
-      </c>
-    </row>
-    <row r="37" spans="1:15" ht="25">
-      <c r="A37" s="1" t="s">
-        <v>512</v>
-      </c>
-      <c r="B37" s="1" t="s">
-        <v>513</v>
-      </c>
-      <c r="C37" s="1" t="s">
-        <v>514</v>
-      </c>
-      <c r="D37" s="1" t="s">
-        <v>515</v>
-      </c>
-      <c r="O37" t="s">
         <v>589</v>
-      </c>
-    </row>
-    <row r="38" spans="1:15" ht="25">
-      <c r="A38" s="1" t="s">
-        <v>516</v>
-      </c>
-      <c r="B38" s="1" t="s">
-        <v>517</v>
-      </c>
-      <c r="C38" s="1" t="s">
-        <v>518</v>
-      </c>
-      <c r="D38" s="1" t="s">
-        <v>519</v>
-      </c>
-      <c r="O38" t="s">
-        <v>590</v>
-      </c>
-    </row>
-    <row r="39" spans="1:15" ht="25">
-      <c r="A39" s="1" t="s">
-        <v>532</v>
-      </c>
-      <c r="B39" s="1" t="s">
-        <v>533</v>
-      </c>
-      <c r="C39" s="1" t="s">
-        <v>534</v>
-      </c>
-      <c r="D39" s="1" t="s">
-        <v>535</v>
-      </c>
-      <c r="O39" t="s">
-        <v>592</v>
-      </c>
-    </row>
-    <row r="40" spans="1:15" ht="25">
-      <c r="A40" s="1" t="s">
-        <v>536</v>
-      </c>
-      <c r="B40" s="1" t="s">
-        <v>537</v>
-      </c>
-      <c r="C40" s="1" t="s">
-        <v>538</v>
-      </c>
-      <c r="D40" s="1" t="s">
-        <v>539</v>
-      </c>
-      <c r="O40" t="s">
-        <v>593</v>
-      </c>
-    </row>
-    <row r="41" spans="1:15" ht="25">
-      <c r="A41" s="1" t="s">
-        <v>322</v>
-      </c>
-      <c r="B41" s="1" t="s">
-        <v>323</v>
-      </c>
-      <c r="C41" s="1" t="s">
-        <v>324</v>
-      </c>
-      <c r="D41" s="1" t="s">
-        <v>325</v>
-      </c>
-      <c r="O41" t="s">
-        <v>594</v>
       </c>
     </row>
   </sheetData>
@@ -3714,1250 +5369,4 @@
     </ext>
   </extLst>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:X85"/>
-  <sheetViews>
-    <sheetView showRuler="0" topLeftCell="A45" workbookViewId="0">
-      <selection activeCell="A85" sqref="A85:XFD85"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
-  <sheetData>
-    <row r="1" spans="1:18" ht="25">
-      <c r="A1" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="2" spans="1:18" ht="25">
-      <c r="A2" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="3" spans="1:18" ht="25">
-      <c r="A3" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="4" spans="1:18" ht="25">
-      <c r="A4" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="L4" t="s">
-        <v>550</v>
-      </c>
-    </row>
-    <row r="5" spans="1:18" ht="25">
-      <c r="A5" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="6" spans="1:18" ht="25">
-      <c r="A6" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="M6" t="s">
-        <v>551</v>
-      </c>
-    </row>
-    <row r="7" spans="1:18" ht="25">
-      <c r="A7" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="Q7" t="s">
-        <v>553</v>
-      </c>
-    </row>
-    <row r="8" spans="1:18" ht="25">
-      <c r="A8" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="9" spans="1:18" ht="25">
-      <c r="A9" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="R9" t="s">
-        <v>553</v>
-      </c>
-    </row>
-    <row r="10" spans="1:18" ht="25">
-      <c r="A10" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="11" spans="1:18" ht="25">
-      <c r="A11" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="12" spans="1:18" ht="25">
-      <c r="A12" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="13" spans="1:18" ht="25">
-      <c r="A13" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="14" spans="1:18" ht="25">
-      <c r="A14" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="M14" t="s">
-        <v>553</v>
-      </c>
-    </row>
-    <row r="15" spans="1:18" ht="25">
-      <c r="A15" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="16" spans="1:18" ht="25">
-      <c r="A16" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>129</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="17" spans="1:24" ht="25">
-      <c r="A17" s="1" t="s">
-        <v>135</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>136</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="D17" s="1" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="18" spans="1:24" ht="25">
-      <c r="A18" s="1" t="s">
-        <v>147</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>148</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>149</v>
-      </c>
-      <c r="D18" s="1" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="19" spans="1:24" ht="25">
-      <c r="A19" s="1" t="s">
-        <v>163</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>164</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>165</v>
-      </c>
-      <c r="D19" s="1" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="20" spans="1:24" ht="25">
-      <c r="A20" s="1" t="s">
-        <v>167</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>168</v>
-      </c>
-      <c r="C20" s="1"/>
-      <c r="D20" s="1" t="s">
-        <v>169</v>
-      </c>
-      <c r="M20" t="s">
-        <v>557</v>
-      </c>
-    </row>
-    <row r="21" spans="1:24" ht="25">
-      <c r="A21" s="1" t="s">
-        <v>174</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>175</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>176</v>
-      </c>
-      <c r="D21" s="1" t="s">
-        <v>177</v>
-      </c>
-      <c r="X21" t="s">
-        <v>560</v>
-      </c>
-    </row>
-    <row r="22" spans="1:24" ht="25">
-      <c r="A22" s="1" t="s">
-        <v>182</v>
-      </c>
-      <c r="B22" s="1" t="s">
-        <v>183</v>
-      </c>
-      <c r="C22" s="1" t="s">
-        <v>184</v>
-      </c>
-      <c r="D22" s="1" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="23" spans="1:24" ht="25">
-      <c r="A23" s="1" t="s">
-        <v>214</v>
-      </c>
-      <c r="B23" s="1" t="s">
-        <v>215</v>
-      </c>
-      <c r="C23" s="1" t="s">
-        <v>216</v>
-      </c>
-      <c r="D23" s="1" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="24" spans="1:24" ht="25">
-      <c r="A24" s="1" t="s">
-        <v>234</v>
-      </c>
-      <c r="B24" s="1" t="s">
-        <v>235</v>
-      </c>
-      <c r="C24" s="1" t="s">
-        <v>236</v>
-      </c>
-      <c r="D24" s="1" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="25" spans="1:24" ht="25">
-      <c r="A25" s="1" t="s">
-        <v>222</v>
-      </c>
-      <c r="B25" s="1" t="s">
-        <v>223</v>
-      </c>
-      <c r="C25" s="1" t="s">
-        <v>224</v>
-      </c>
-      <c r="D25" s="1" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="26" spans="1:24" ht="25">
-      <c r="A26" s="1" t="s">
-        <v>230</v>
-      </c>
-      <c r="B26" s="1" t="s">
-        <v>231</v>
-      </c>
-      <c r="C26" s="1" t="s">
-        <v>232</v>
-      </c>
-      <c r="D26" s="1" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="27" spans="1:24" ht="25">
-      <c r="A27" s="1" t="s">
-        <v>242</v>
-      </c>
-      <c r="B27" s="1" t="s">
-        <v>243</v>
-      </c>
-      <c r="C27" s="1" t="s">
-        <v>244</v>
-      </c>
-      <c r="D27" s="1" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="28" spans="1:24" ht="25">
-      <c r="A28" s="1" t="s">
-        <v>254</v>
-      </c>
-      <c r="B28" s="1" t="s">
-        <v>255</v>
-      </c>
-      <c r="C28" s="1" t="s">
-        <v>256</v>
-      </c>
-      <c r="D28" s="1" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="29" spans="1:24" ht="25">
-      <c r="A29" s="1" t="s">
-        <v>258</v>
-      </c>
-      <c r="B29" s="1" t="s">
-        <v>259</v>
-      </c>
-      <c r="C29" s="1" t="s">
-        <v>260</v>
-      </c>
-      <c r="D29" s="1" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="30" spans="1:24" ht="25">
-      <c r="A30" s="1" t="s">
-        <v>262</v>
-      </c>
-      <c r="B30" s="1" t="s">
-        <v>263</v>
-      </c>
-      <c r="C30" s="1" t="s">
-        <v>264</v>
-      </c>
-      <c r="D30" s="1" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="31" spans="1:24" ht="25">
-      <c r="A31" s="1" t="s">
-        <v>270</v>
-      </c>
-      <c r="B31" s="1" t="s">
-        <v>271</v>
-      </c>
-      <c r="C31" s="1" t="s">
-        <v>272</v>
-      </c>
-      <c r="D31" s="1" t="s">
-        <v>273</v>
-      </c>
-    </row>
-    <row r="32" spans="1:24" ht="25">
-      <c r="A32" s="1" t="s">
-        <v>274</v>
-      </c>
-      <c r="B32" s="1" t="s">
-        <v>275</v>
-      </c>
-      <c r="C32" s="1" t="s">
-        <v>276</v>
-      </c>
-      <c r="D32" s="1" t="s">
-        <v>277</v>
-      </c>
-    </row>
-    <row r="33" spans="1:12" ht="25">
-      <c r="A33" s="1" t="s">
-        <v>278</v>
-      </c>
-      <c r="B33" s="1" t="s">
-        <v>279</v>
-      </c>
-      <c r="C33" s="1" t="s">
-        <v>280</v>
-      </c>
-      <c r="D33" s="1" t="s">
-        <v>281</v>
-      </c>
-    </row>
-    <row r="34" spans="1:12" ht="25">
-      <c r="A34" s="1" t="s">
-        <v>282</v>
-      </c>
-      <c r="B34" s="1" t="s">
-        <v>283</v>
-      </c>
-      <c r="C34" s="1" t="s">
-        <v>284</v>
-      </c>
-      <c r="D34" s="1" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="35" spans="1:12" ht="25">
-      <c r="A35" s="1" t="s">
-        <v>290</v>
-      </c>
-      <c r="B35" s="1" t="s">
-        <v>291</v>
-      </c>
-      <c r="C35" s="1" t="s">
-        <v>292</v>
-      </c>
-      <c r="D35" s="1" t="s">
-        <v>293</v>
-      </c>
-      <c r="L35" t="s">
-        <v>574</v>
-      </c>
-    </row>
-    <row r="36" spans="1:12" ht="25">
-      <c r="A36" s="1" t="s">
-        <v>306</v>
-      </c>
-      <c r="B36" s="1" t="s">
-        <v>307</v>
-      </c>
-      <c r="C36" s="1" t="s">
-        <v>308</v>
-      </c>
-      <c r="D36" s="1" t="s">
-        <v>309</v>
-      </c>
-    </row>
-    <row r="37" spans="1:12" ht="25">
-      <c r="A37" s="1" t="s">
-        <v>310</v>
-      </c>
-      <c r="B37" s="1" t="s">
-        <v>311</v>
-      </c>
-      <c r="C37" s="1" t="s">
-        <v>312</v>
-      </c>
-      <c r="D37" s="1" t="s">
-        <v>313</v>
-      </c>
-    </row>
-    <row r="38" spans="1:12" ht="25">
-      <c r="A38" s="1" t="s">
-        <v>318</v>
-      </c>
-      <c r="B38" s="1" t="s">
-        <v>319</v>
-      </c>
-      <c r="C38" s="1" t="s">
-        <v>320</v>
-      </c>
-      <c r="D38" s="1" t="s">
-        <v>321</v>
-      </c>
-    </row>
-    <row r="39" spans="1:12" ht="25">
-      <c r="A39" s="1" t="s">
-        <v>338</v>
-      </c>
-      <c r="B39" s="1" t="s">
-        <v>339</v>
-      </c>
-      <c r="C39" s="1" t="s">
-        <v>340</v>
-      </c>
-      <c r="D39" s="1" t="s">
-        <v>341</v>
-      </c>
-    </row>
-    <row r="40" spans="1:12" ht="25">
-      <c r="A40" s="1" t="s">
-        <v>334</v>
-      </c>
-      <c r="B40" s="1" t="s">
-        <v>335</v>
-      </c>
-      <c r="C40" s="1" t="s">
-        <v>336</v>
-      </c>
-      <c r="D40" s="1" t="s">
-        <v>337</v>
-      </c>
-    </row>
-    <row r="41" spans="1:12" ht="25">
-      <c r="A41" s="1" t="s">
-        <v>342</v>
-      </c>
-      <c r="B41" s="1" t="s">
-        <v>343</v>
-      </c>
-      <c r="C41" s="1" t="s">
-        <v>344</v>
-      </c>
-      <c r="D41" s="1" t="s">
-        <v>345</v>
-      </c>
-    </row>
-    <row r="42" spans="1:12" ht="25">
-      <c r="A42" s="1" t="s">
-        <v>346</v>
-      </c>
-      <c r="B42" s="1" t="s">
-        <v>347</v>
-      </c>
-      <c r="C42" s="1" t="s">
-        <v>348</v>
-      </c>
-      <c r="D42" s="1" t="s">
-        <v>349</v>
-      </c>
-    </row>
-    <row r="43" spans="1:12" ht="25">
-      <c r="A43" s="1" t="s">
-        <v>350</v>
-      </c>
-      <c r="B43" s="1" t="s">
-        <v>351</v>
-      </c>
-      <c r="C43" s="1" t="s">
-        <v>352</v>
-      </c>
-      <c r="D43" s="1" t="s">
-        <v>353</v>
-      </c>
-    </row>
-    <row r="44" spans="1:12" ht="25">
-      <c r="A44" s="1" t="s">
-        <v>362</v>
-      </c>
-      <c r="B44" s="1" t="s">
-        <v>363</v>
-      </c>
-      <c r="C44" s="1" t="s">
-        <v>364</v>
-      </c>
-      <c r="D44" s="1" t="s">
-        <v>365</v>
-      </c>
-    </row>
-    <row r="45" spans="1:12" ht="25">
-      <c r="A45" s="1" t="s">
-        <v>366</v>
-      </c>
-      <c r="B45" s="1" t="s">
-        <v>367</v>
-      </c>
-      <c r="C45" s="1" t="s">
-        <v>368</v>
-      </c>
-      <c r="D45" s="1" t="s">
-        <v>369</v>
-      </c>
-    </row>
-    <row r="46" spans="1:12" ht="25">
-      <c r="A46" s="1" t="s">
-        <v>378</v>
-      </c>
-      <c r="B46" s="1" t="s">
-        <v>379</v>
-      </c>
-      <c r="C46" s="1" t="s">
-        <v>380</v>
-      </c>
-      <c r="D46" s="1" t="s">
-        <v>381</v>
-      </c>
-    </row>
-    <row r="47" spans="1:12" ht="25">
-      <c r="A47" s="1" t="s">
-        <v>382</v>
-      </c>
-      <c r="B47" s="1" t="s">
-        <v>383</v>
-      </c>
-      <c r="C47" s="1" t="s">
-        <v>384</v>
-      </c>
-      <c r="D47" s="1" t="s">
-        <v>385</v>
-      </c>
-    </row>
-    <row r="48" spans="1:12" ht="25">
-      <c r="A48" s="1" t="s">
-        <v>390</v>
-      </c>
-      <c r="B48" s="1" t="s">
-        <v>391</v>
-      </c>
-      <c r="C48" s="1" t="s">
-        <v>392</v>
-      </c>
-      <c r="D48" s="1" t="s">
-        <v>393</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4" ht="25">
-      <c r="A49" s="1" t="s">
-        <v>398</v>
-      </c>
-      <c r="B49" s="1" t="s">
-        <v>399</v>
-      </c>
-      <c r="C49" s="1" t="s">
-        <v>400</v>
-      </c>
-      <c r="D49" s="1" t="s">
-        <v>401</v>
-      </c>
-    </row>
-    <row r="50" spans="1:4" ht="25">
-      <c r="A50" s="1" t="s">
-        <v>402</v>
-      </c>
-      <c r="B50" s="1" t="s">
-        <v>403</v>
-      </c>
-      <c r="C50" s="1" t="s">
-        <v>404</v>
-      </c>
-      <c r="D50" s="1" t="s">
-        <v>405</v>
-      </c>
-    </row>
-    <row r="51" spans="1:4" ht="25">
-      <c r="A51" s="1" t="s">
-        <v>406</v>
-      </c>
-      <c r="B51" s="1" t="s">
-        <v>407</v>
-      </c>
-      <c r="C51" s="1" t="s">
-        <v>408</v>
-      </c>
-      <c r="D51" s="1" t="s">
-        <v>409</v>
-      </c>
-    </row>
-    <row r="52" spans="1:4" ht="25">
-      <c r="A52" s="1" t="s">
-        <v>414</v>
-      </c>
-      <c r="B52" s="1" t="s">
-        <v>415</v>
-      </c>
-      <c r="C52" s="1" t="s">
-        <v>416</v>
-      </c>
-      <c r="D52" s="1" t="s">
-        <v>417</v>
-      </c>
-    </row>
-    <row r="53" spans="1:4" ht="25">
-      <c r="A53" s="1" t="s">
-        <v>422</v>
-      </c>
-      <c r="B53" s="1" t="s">
-        <v>423</v>
-      </c>
-      <c r="C53" s="1" t="s">
-        <v>424</v>
-      </c>
-      <c r="D53" s="1" t="s">
-        <v>425</v>
-      </c>
-    </row>
-    <row r="54" spans="1:4" ht="25">
-      <c r="A54" s="1" t="s">
-        <v>426</v>
-      </c>
-      <c r="B54" s="1" t="s">
-        <v>427</v>
-      </c>
-      <c r="C54" s="1" t="s">
-        <v>428</v>
-      </c>
-      <c r="D54" s="1" t="s">
-        <v>429</v>
-      </c>
-    </row>
-    <row r="55" spans="1:4" ht="25">
-      <c r="A55" s="1" t="s">
-        <v>433</v>
-      </c>
-      <c r="B55" s="1" t="s">
-        <v>434</v>
-      </c>
-      <c r="C55" s="1" t="s">
-        <v>435</v>
-      </c>
-      <c r="D55" s="1" t="s">
-        <v>436</v>
-      </c>
-    </row>
-    <row r="56" spans="1:4" ht="25">
-      <c r="A56" s="1" t="s">
-        <v>445</v>
-      </c>
-      <c r="B56" s="1" t="s">
-        <v>446</v>
-      </c>
-      <c r="C56" s="1" t="s">
-        <v>447</v>
-      </c>
-      <c r="D56" s="1" t="s">
-        <v>448</v>
-      </c>
-    </row>
-    <row r="57" spans="1:4" ht="25">
-      <c r="A57" s="1" t="s">
-        <v>453</v>
-      </c>
-      <c r="B57" s="1" t="s">
-        <v>454</v>
-      </c>
-      <c r="C57" s="1" t="s">
-        <v>455</v>
-      </c>
-      <c r="D57" s="1" t="s">
-        <v>456</v>
-      </c>
-    </row>
-    <row r="58" spans="1:4" ht="25">
-      <c r="A58" s="1" t="s">
-        <v>457</v>
-      </c>
-      <c r="B58" s="1" t="s">
-        <v>458</v>
-      </c>
-      <c r="C58" s="1" t="s">
-        <v>459</v>
-      </c>
-      <c r="D58" s="1" t="s">
-        <v>460</v>
-      </c>
-    </row>
-    <row r="59" spans="1:4" ht="25">
-      <c r="A59" s="1" t="s">
-        <v>461</v>
-      </c>
-      <c r="B59" s="1" t="s">
-        <v>462</v>
-      </c>
-      <c r="C59" s="1" t="s">
-        <v>463</v>
-      </c>
-      <c r="D59" s="1" t="s">
-        <v>464</v>
-      </c>
-    </row>
-    <row r="60" spans="1:4" ht="25">
-      <c r="A60" s="1" t="s">
-        <v>465</v>
-      </c>
-      <c r="B60" s="1" t="s">
-        <v>466</v>
-      </c>
-      <c r="C60" s="1" t="s">
-        <v>467</v>
-      </c>
-      <c r="D60" s="1" t="s">
-        <v>468</v>
-      </c>
-    </row>
-    <row r="61" spans="1:4" ht="25">
-      <c r="A61" s="1" t="s">
-        <v>473</v>
-      </c>
-      <c r="B61" s="1" t="s">
-        <v>474</v>
-      </c>
-      <c r="C61" s="1" t="s">
-        <v>475</v>
-      </c>
-      <c r="D61" s="1" t="s">
-        <v>476</v>
-      </c>
-    </row>
-    <row r="62" spans="1:4" ht="25">
-      <c r="A62" s="1" t="s">
-        <v>477</v>
-      </c>
-      <c r="B62" s="1" t="s">
-        <v>478</v>
-      </c>
-      <c r="C62" s="1"/>
-      <c r="D62" s="1" t="s">
-        <v>479</v>
-      </c>
-    </row>
-    <row r="63" spans="1:4" ht="25">
-      <c r="A63" s="1" t="s">
-        <v>480</v>
-      </c>
-      <c r="B63" s="1" t="s">
-        <v>481</v>
-      </c>
-      <c r="C63" s="1" t="s">
-        <v>482</v>
-      </c>
-      <c r="D63" s="1" t="s">
-        <v>483</v>
-      </c>
-    </row>
-    <row r="64" spans="1:4" ht="25">
-      <c r="A64" s="1" t="s">
-        <v>484</v>
-      </c>
-      <c r="B64" s="1" t="s">
-        <v>485</v>
-      </c>
-      <c r="C64" s="1" t="s">
-        <v>486</v>
-      </c>
-      <c r="D64" s="1" t="s">
-        <v>487</v>
-      </c>
-    </row>
-    <row r="65" spans="1:4" ht="25">
-      <c r="A65" s="1" t="s">
-        <v>492</v>
-      </c>
-      <c r="B65" s="1" t="s">
-        <v>493</v>
-      </c>
-      <c r="C65" s="1" t="s">
-        <v>494</v>
-      </c>
-      <c r="D65" s="1" t="s">
-        <v>495</v>
-      </c>
-    </row>
-    <row r="66" spans="1:4" ht="25">
-      <c r="A66" s="1" t="s">
-        <v>500</v>
-      </c>
-      <c r="B66" s="1" t="s">
-        <v>501</v>
-      </c>
-      <c r="C66" s="1" t="s">
-        <v>502</v>
-      </c>
-      <c r="D66" s="1" t="s">
-        <v>503</v>
-      </c>
-    </row>
-    <row r="67" spans="1:4" ht="25">
-      <c r="A67" s="1" t="s">
-        <v>508</v>
-      </c>
-      <c r="B67" s="1" t="s">
-        <v>509</v>
-      </c>
-      <c r="C67" s="1" t="s">
-        <v>510</v>
-      </c>
-      <c r="D67" s="1" t="s">
-        <v>511</v>
-      </c>
-    </row>
-    <row r="68" spans="1:4" ht="25">
-      <c r="A68" s="1" t="s">
-        <v>524</v>
-      </c>
-      <c r="B68" s="1" t="s">
-        <v>525</v>
-      </c>
-      <c r="C68" s="1" t="s">
-        <v>526</v>
-      </c>
-      <c r="D68" s="1" t="s">
-        <v>527</v>
-      </c>
-    </row>
-    <row r="69" spans="1:4" ht="25">
-      <c r="A69" s="1" t="s">
-        <v>528</v>
-      </c>
-      <c r="B69" s="1" t="s">
-        <v>529</v>
-      </c>
-      <c r="C69" s="1" t="s">
-        <v>530</v>
-      </c>
-      <c r="D69" s="1" t="s">
-        <v>531</v>
-      </c>
-    </row>
-    <row r="70" spans="1:4" ht="25">
-      <c r="A70" s="1" t="s">
-        <v>540</v>
-      </c>
-      <c r="B70" s="1" t="s">
-        <v>541</v>
-      </c>
-      <c r="C70" s="1" t="s">
-        <v>542</v>
-      </c>
-      <c r="D70" s="1" t="s">
-        <v>543</v>
-      </c>
-    </row>
-    <row r="71" spans="1:4" ht="25">
-      <c r="A71" s="1" t="s">
-        <v>544</v>
-      </c>
-      <c r="B71" s="1" t="s">
-        <v>545</v>
-      </c>
-      <c r="C71" s="1" t="s">
-        <v>546</v>
-      </c>
-      <c r="D71" s="1" t="s">
-        <v>547</v>
-      </c>
-    </row>
-    <row r="72" spans="1:4" ht="25">
-      <c r="A72" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B72" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C72" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D72" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="73" spans="1:4" ht="25">
-      <c r="A73" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B73" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C73" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D73" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="74" spans="1:4" ht="25">
-      <c r="A74" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="B74" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="C74" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="D74" s="1" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="75" spans="1:4" ht="25">
-      <c r="A75" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="B75" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="C75" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="D75" s="1" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="76" spans="1:4" ht="25">
-      <c r="A76" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="B76" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="C76" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="D76" s="1" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="77" spans="1:4" ht="25">
-      <c r="A77" s="1" t="s">
-        <v>139</v>
-      </c>
-      <c r="B77" s="1" t="s">
-        <v>140</v>
-      </c>
-      <c r="C77" s="1" t="s">
-        <v>141</v>
-      </c>
-      <c r="D77" s="1" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="78" spans="1:4" ht="25">
-      <c r="A78" s="1" t="s">
-        <v>170</v>
-      </c>
-      <c r="B78" s="1" t="s">
-        <v>171</v>
-      </c>
-      <c r="C78" s="1" t="s">
-        <v>172</v>
-      </c>
-      <c r="D78" s="1" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="79" spans="1:4" ht="25">
-      <c r="A79" s="1" t="s">
-        <v>178</v>
-      </c>
-      <c r="B79" s="1" t="s">
-        <v>179</v>
-      </c>
-      <c r="C79" s="1" t="s">
-        <v>180</v>
-      </c>
-      <c r="D79" s="1" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="80" spans="1:4" ht="25">
-      <c r="A80" s="1" t="s">
-        <v>354</v>
-      </c>
-      <c r="B80" s="1" t="s">
-        <v>355</v>
-      </c>
-      <c r="C80" s="1" t="s">
-        <v>356</v>
-      </c>
-      <c r="D80" s="1" t="s">
-        <v>357</v>
-      </c>
-    </row>
-    <row r="81" spans="1:12" ht="25">
-      <c r="A81" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="B81" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="C81" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="D81" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="L81" t="s">
-        <v>555</v>
-      </c>
-    </row>
-    <row r="82" spans="1:12" ht="25">
-      <c r="A82" s="1" t="s">
-        <v>131</v>
-      </c>
-      <c r="B82" s="1" t="s">
-        <v>132</v>
-      </c>
-      <c r="C82" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="D82" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="L82" t="s">
-        <v>555</v>
-      </c>
-    </row>
-    <row r="83" spans="1:12" ht="25">
-      <c r="A83" s="1" t="s">
-        <v>155</v>
-      </c>
-      <c r="B83" s="1" t="s">
-        <v>156</v>
-      </c>
-      <c r="C83" s="1" t="s">
-        <v>157</v>
-      </c>
-      <c r="D83" s="1" t="s">
-        <v>158</v>
-      </c>
-      <c r="L83" t="s">
-        <v>555</v>
-      </c>
-    </row>
-    <row r="84" spans="1:12" ht="25">
-      <c r="A84" s="1" t="s">
-        <v>358</v>
-      </c>
-      <c r="B84" s="1" t="s">
-        <v>359</v>
-      </c>
-      <c r="C84" s="1" t="s">
-        <v>360</v>
-      </c>
-      <c r="D84" s="1" t="s">
-        <v>361</v>
-      </c>
-      <c r="L84" t="s">
-        <v>581</v>
-      </c>
-    </row>
-    <row r="85" spans="1:12" ht="25">
-      <c r="A85" s="1" t="s">
-        <v>469</v>
-      </c>
-      <c r="B85" s="1" t="s">
-        <v>470</v>
-      </c>
-      <c r="C85" s="1" t="s">
-        <v>471</v>
-      </c>
-      <c r="D85" s="1" t="s">
-        <v>472</v>
-      </c>
-      <c r="L85" t="s">
-        <v>581</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
-</worksheet>
 </file>
</xml_diff>